<commit_message>
refactor bearing calculations and enhance chain force computation
</commit_message>
<xml_diff>
--- a/Bearing Choices.xlsx
+++ b/Bearing Choices.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsoep\OUR\Bearing_Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA675A3F-B989-4D3E-A455-4288D298A798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7DE4E1-F35E-4ABA-BA41-B4A36DC508C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bearing choices" sheetId="1" r:id="rId1"/>
+    <sheet name="bearing distances" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>https://www.skf.com/uk/products/rolling-bearings/ball-bearings/deep-groove-ball-bearings/productid-6407%2FC3</t>
   </si>
@@ -91,13 +103,46 @@
   </si>
   <si>
     <t>Dynamic Load Rating (kN)</t>
+  </si>
+  <si>
+    <t>bearing</t>
+  </si>
+  <si>
+    <t>sprocket width</t>
+  </si>
+  <si>
+    <t>bearing width</t>
+  </si>
+  <si>
+    <t>min dist</t>
+  </si>
+  <si>
+    <t>A (near)</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>SKF 3207 A 2RS1</t>
+  </si>
+  <si>
+    <t>B (far)</t>
+  </si>
+  <si>
+    <t>SKF 6306 2RS1</t>
+  </si>
+  <si>
+    <t>midplane dist</t>
+  </si>
+  <si>
+    <t>motor spline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +157,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -284,27 +335,30 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF666666"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -442,6 +496,22 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -458,18 +528,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}" name="Table1" displayName="Table1" ref="B2:J7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}" name="Table1" displayName="Table1" ref="B2:J7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="B2:J7" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E0BE4D0C-B5A6-46B3-8638-696A5E4206A8}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{A1E4B19A-F452-426B-8DC1-720CCEC36229}" name="Link" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{A1E4B19A-F452-426B-8DC1-720CCEC36229}" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{13AD953A-3BD3-4E61-852E-84A9C66CA948}" name="Bearing type"/>
-    <tableColumn id="4" xr3:uid="{CD905FA5-831F-4023-AC95-3F34A8A3B833}" name="Static Load Rating (kN)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{76782C9D-0919-4703-B3B3-2A87424F3B1B}" name="Dynamic Load Rating (kN)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{05711982-53CE-46B5-841A-867B8BAE93A9}" name="Bore Diameter (mm)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4D8F94C2-8A0D-45EC-B127-F7B5840E943E}" name="Outside Diameter (mm)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{F656D5A9-FF5B-46D4-A398-19949ECC5254}" name="Width (mm)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{EA7A9A09-B23D-4A4A-94D9-9166880E4840}" name="Limiting Speed (rpm)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CD905FA5-831F-4023-AC95-3F34A8A3B833}" name="Static Load Rating (kN)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{76782C9D-0919-4703-B3B3-2A87424F3B1B}" name="Dynamic Load Rating (kN)" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{05711982-53CE-46B5-841A-867B8BAE93A9}" name="Bore Diameter (mm)" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{4D8F94C2-8A0D-45EC-B127-F7B5840E943E}" name="Outside Diameter (mm)" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{F656D5A9-FF5B-46D4-A398-19949ECC5254}" name="Width (mm)" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{EA7A9A09-B23D-4A4A-94D9-9166880E4840}" name="Limiting Speed (rpm)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49C8949E-B2E7-472D-A72E-E8F6764E377C}" name="Table2" displayName="Table2" ref="A1:F4" totalsRowShown="0">
+  <autoFilter ref="A1:F4" xr:uid="{49C8949E-B2E7-472D-A72E-E8F6764E377C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D82E3139-CC35-4EF9-9F8B-A5398B13C79E}" name="bearing"/>
+    <tableColumn id="2" xr3:uid="{1D1CAE33-1669-4971-8A4B-B1AFF07E19F2}" name="model"/>
+    <tableColumn id="3" xr3:uid="{4C85C1B7-3CAC-4CA0-AF5B-8FD2373E9263}" name="sprocket width"/>
+    <tableColumn id="4" xr3:uid="{46C74B83-2E01-4B4B-840C-8666E21995CE}" name="bearing width"/>
+    <tableColumn id="5" xr3:uid="{4FBB8988-31A1-4948-8F3B-C45942DE91AE}" name="min dist" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F02AF1CD-2A1B-48CD-B23D-DFD4A3A771EA}" name="midplane dist"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1105,4 +1190,108 @@
     <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1909DA-F803-4A95-BDC3-3A661989B98E}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>12.826000000000001</v>
+      </c>
+      <c r="D2">
+        <v>27</v>
+      </c>
+      <c r="E2" s="16">
+        <v>30.378</v>
+      </c>
+      <c r="F2">
+        <f>E2+D2/2+C2</f>
+        <v>56.704000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>12.826000000000001</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3" s="16">
+        <v>167.078</v>
+      </c>
+      <c r="F3">
+        <f>E3+D3/2+C3</f>
+        <v>189.404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>12.826000000000001</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4" s="16">
+        <v>82.878</v>
+      </c>
+      <c r="F4">
+        <f>E4+D4+C4</f>
+        <v>143.70399999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new shaft material, fixed chain force computation, updated bearing list
</commit_message>
<xml_diff>
--- a/Bearing Choices.xlsx
+++ b/Bearing Choices.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsoep\OUR\Bearing_Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7DE4E1-F35E-4ABA-BA41-B4A36DC508C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB01C1-6F36-4B63-9029-E304817BCF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bearing choices" sheetId="1" r:id="rId1"/>
-    <sheet name="bearing distances" sheetId="2" r:id="rId2"/>
+    <sheet name="bearing choices" sheetId="3" r:id="rId1"/>
+    <sheet name="bearing choices old" sheetId="1" r:id="rId2"/>
+    <sheet name="bearing distances" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>https://www.skf.com/uk/products/rolling-bearings/ball-bearings/deep-groove-ball-bearings/productid-6407%2FC3</t>
   </si>
@@ -136,13 +137,139 @@
   </si>
   <si>
     <t>motor spline</t>
+  </si>
+  <si>
+    <t>Bearing model</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>Basic load rating (kN)</t>
+  </si>
+  <si>
+    <t>calculated load from Matlab script (kN)</t>
+  </si>
+  <si>
+    <t>SF = C0 / calc load</t>
+  </si>
+  <si>
+    <t>bore aka ID</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>dynamic C (should be irrelevant)</t>
+  </si>
+  <si>
+    <t>static C0</t>
+  </si>
+  <si>
+    <t>SKF website</t>
+  </si>
+  <si>
+    <t>double row angular contact with contact seals</t>
+  </si>
+  <si>
+    <t>We already have this – used in OUR1-4 gearbox and we have spares</t>
+  </si>
+  <si>
+    <t>SKF 6306-2RS1</t>
+  </si>
+  <si>
+    <t>single row deep groove with contact seals</t>
+  </si>
+  <si>
+    <t>RS: 14.15 ex VAT</t>
+  </si>
+  <si>
+    <t>SKF website link</t>
+  </si>
+  <si>
+    <t>Where to buy</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Bearing location</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Price ex VAT</t>
+  </si>
+  <si>
+    <t>SKF 3307 A-2RS1TN9/MT33</t>
+  </si>
+  <si>
+    <t>https://www.skf.com/group/products/rolling-bearings/ball-bearings/angular-contact-ball-bearings/double-row-angular-contact-ball-bearings/productid-3307%20A-2RS1TN9%2FMT33</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/ball-bearings/1959546</t>
+  </si>
+  <si>
+    <t>SKF 3207 A-2RS1TN9/MT33</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/ball-bearings/0505625</t>
+  </si>
+  <si>
+    <t>3206 A-2RS1TN9/MT33</t>
+  </si>
+  <si>
+    <t>https://www.skf.com/group/products/rolling-bearings/ball-bearings/angular-contact-ball-bearings/double-row-angular-contact-ball-bearings/productid-3206%20A-2RS1TN9%2FMT33</t>
+  </si>
+  <si>
+    <t>https://www.skf.com/group/products/rolling-bearings/ball-bearings/angular-contact-ball-bearings/double-row-angular-contact-ball-bearings/productid-3207%20A-2RS1TN9%2FMT33</t>
+  </si>
+  <si>
+    <t>max rpm (must &gt;=6100)</t>
+  </si>
+  <si>
+    <t>SKF 3307 A-2ZTN9/MT33</t>
+  </si>
+  <si>
+    <t>double row angular contact with shield</t>
+  </si>
+  <si>
+    <t>https://www.skf.com/group/products/rolling-bearings/ball-bearings/angular-contact-ball-bearings/double-row-angular-contact-ball-bearings/productid-3307%20A-2ZTN9%2FMT33</t>
+  </si>
+  <si>
+    <t>https://www.bearings-online.co.uk/item/5389/SKF/3307A-2ZTN9MT33-SKF.html</t>
+  </si>
+  <si>
+    <t>in CAD</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/ball-bearings/1959544</t>
+  </si>
+  <si>
+    <t>SKF 3306 A-2RS1TN9/MT33</t>
+  </si>
+  <si>
+    <t>https://www.skf.com/group/products/rolling-bearings/ball-bearings/angular-contact-ball-bearings/double-row-angular-contact-ball-bearings/productid-3306%20A-2RS1TN9%2FMT33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +286,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF666666"/>
-      <name val="Arial"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +311,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -335,13 +477,196 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="25">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -353,166 +678,281 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF666666"/>
-        <name val="Arial"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -528,24 +968,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}" name="Table1" displayName="Table1" ref="B2:J7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="B2:J7" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E0BE4D0C-B5A6-46B3-8638-696A5E4206A8}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{A1E4B19A-F452-426B-8DC1-720CCEC36229}" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{13AD953A-3BD3-4E61-852E-84A9C66CA948}" name="Bearing type"/>
-    <tableColumn id="4" xr3:uid="{CD905FA5-831F-4023-AC95-3F34A8A3B833}" name="Static Load Rating (kN)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{76782C9D-0919-4703-B3B3-2A87424F3B1B}" name="Dynamic Load Rating (kN)" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{05711982-53CE-46B5-841A-867B8BAE93A9}" name="Bore Diameter (mm)" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{4D8F94C2-8A0D-45EC-B127-F7B5840E943E}" name="Outside Diameter (mm)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F656D5A9-FF5B-46D4-A398-19949ECC5254}" name="Width (mm)" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{EA7A9A09-B23D-4A4A-94D9-9166880E4840}" name="Limiting Speed (rpm)" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D42E6DD3-13AC-4518-996F-F66AC6704BCA}" name="Table3" displayName="Table3" ref="A2:O8" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A2:O8" xr:uid="{D42E6DD3-13AC-4518-996F-F66AC6704BCA}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{D3D7D069-2358-43B4-8BF5-E55AAD7557FD}" name="Bearing location"/>
+    <tableColumn id="2" xr3:uid="{49A489A2-EC81-479C-9B65-A11A84668A70}" name="Bearing model" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{FCFA3468-5A59-4B6B-9196-B443FEEFEA1C}" name="Description" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{D2932FF7-19F7-4B4E-8C7D-BFAEACE5466E}" name="SKF website link" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" xr3:uid="{FAEB511F-EF7A-40F1-83F4-5C44D037B700}" name="Where to buy"/>
+    <tableColumn id="6" xr3:uid="{41F99E36-D2F1-40CF-9568-5A392119BFD0}" name="Price ex VAT" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{CFFDAADE-5651-4EA1-9FAC-3E9181ABB5BA}" name="bore aka ID" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{A7F303CD-2D4F-4330-8842-47A1035CEB73}" name="OD" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{56A4A052-17CC-4389-BCA6-E2E950A934C0}" name="width" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{D79B48E1-E61B-4CB9-960B-BE369B215068}" name="dynamic C (should be irrelevant)" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{B2559FEA-B43C-41F4-B1C6-2E253C00C033}" name="static C0" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{B05BB3D7-A9D1-4EB6-BC3C-C0E12C8F84A1}" name="calculated load from Matlab script (kN)" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{6E5645AF-3FFF-4754-8AB4-E161D98C58B8}" name="SF = C0 / calc load" dataDxfId="12">
+      <calculatedColumnFormula>K3/L3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{5FDE3D16-41B3-4120-B965-F9EE3BDDE016}" name="max rpm (must &gt;=6100)" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{DD42C261-BCE4-404C-8DE1-2AAD95FAC9CE}" name="remarks" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}" name="Table1" displayName="Table1" ref="B2:J7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B2:J7" xr:uid="{390CC8AC-5724-4AFD-A5DE-858968EC1B23}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{E0BE4D0C-B5A6-46B3-8638-696A5E4206A8}" name="Model"/>
+    <tableColumn id="2" xr3:uid="{A1E4B19A-F452-426B-8DC1-720CCEC36229}" name="Link" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{13AD953A-3BD3-4E61-852E-84A9C66CA948}" name="Bearing type"/>
+    <tableColumn id="4" xr3:uid="{CD905FA5-831F-4023-AC95-3F34A8A3B833}" name="Static Load Rating (kN)" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{76782C9D-0919-4703-B3B3-2A87424F3B1B}" name="Dynamic Load Rating (kN)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{05711982-53CE-46B5-841A-867B8BAE93A9}" name="Bore Diameter (mm)" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{4D8F94C2-8A0D-45EC-B127-F7B5840E943E}" name="Outside Diameter (mm)" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F656D5A9-FF5B-46D4-A398-19949ECC5254}" name="Width (mm)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{EA7A9A09-B23D-4A4A-94D9-9166880E4840}" name="Limiting Speed (rpm)" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49C8949E-B2E7-472D-A72E-E8F6764E377C}" name="Table2" displayName="Table2" ref="A1:F4" totalsRowShown="0">
   <autoFilter ref="A1:F4" xr:uid="{49C8949E-B2E7-472D-A72E-E8F6764E377C}"/>
   <tableColumns count="6">
@@ -553,7 +1019,7 @@
     <tableColumn id="2" xr3:uid="{1D1CAE33-1669-4971-8A4B-B1AFF07E19F2}" name="model"/>
     <tableColumn id="3" xr3:uid="{4C85C1B7-3CAC-4CA0-AF5B-8FD2373E9263}" name="sprocket width"/>
     <tableColumn id="4" xr3:uid="{46C74B83-2E01-4B4B-840C-8666E21995CE}" name="bearing width"/>
-    <tableColumn id="5" xr3:uid="{4FBB8988-31A1-4948-8F3B-C45942DE91AE}" name="min dist" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{4FBB8988-31A1-4948-8F3B-C45942DE91AE}" name="min dist"/>
     <tableColumn id="6" xr3:uid="{F02AF1CD-2A1B-48CD-B23D-DFD4A3A771EA}" name="midplane dist"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -822,11 +1288,410 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D89061-B20F-468F-AF91-469D4018105C}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" customWidth="1"/>
+    <col min="14" max="14" width="8.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="20">
+        <v>62.28</v>
+      </c>
+      <c r="G3" s="17">
+        <v>35</v>
+      </c>
+      <c r="H3" s="17">
+        <v>80</v>
+      </c>
+      <c r="I3" s="17">
+        <v>34.9</v>
+      </c>
+      <c r="J3" s="17">
+        <v>54</v>
+      </c>
+      <c r="K3" s="17">
+        <v>38</v>
+      </c>
+      <c r="L3" s="17">
+        <v>10.922800000000001</v>
+      </c>
+      <c r="M3" s="22">
+        <f>K3/L3</f>
+        <v>3.4789614384590029</v>
+      </c>
+      <c r="N3" s="17">
+        <v>8500</v>
+      </c>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="20">
+        <v>118.11</v>
+      </c>
+      <c r="G4" s="17">
+        <v>35</v>
+      </c>
+      <c r="H4" s="17">
+        <v>80</v>
+      </c>
+      <c r="I4" s="17">
+        <v>34.9</v>
+      </c>
+      <c r="J4" s="17">
+        <v>54</v>
+      </c>
+      <c r="K4" s="17">
+        <v>38</v>
+      </c>
+      <c r="L4" s="17">
+        <v>10.922800000000001</v>
+      </c>
+      <c r="M4" s="22">
+        <f>K4/L4</f>
+        <v>3.4789614384590029</v>
+      </c>
+      <c r="N4" s="17">
+        <v>6000</v>
+      </c>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="20">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="G5" s="17">
+        <v>35</v>
+      </c>
+      <c r="H5" s="17">
+        <v>72</v>
+      </c>
+      <c r="I5" s="17">
+        <v>27</v>
+      </c>
+      <c r="J5" s="17">
+        <v>40.5</v>
+      </c>
+      <c r="K5" s="17">
+        <v>30</v>
+      </c>
+      <c r="L5" s="17">
+        <v>10.922800000000001</v>
+      </c>
+      <c r="M5" s="22">
+        <f>K5/L5</f>
+        <v>2.7465485040465811</v>
+      </c>
+      <c r="N5" s="17">
+        <v>6300</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="20">
+        <v>100.9</v>
+      </c>
+      <c r="G6" s="17">
+        <v>30</v>
+      </c>
+      <c r="H6" s="17">
+        <v>72</v>
+      </c>
+      <c r="I6" s="17">
+        <v>30.2</v>
+      </c>
+      <c r="J6" s="17">
+        <v>42.5</v>
+      </c>
+      <c r="K6" s="17">
+        <v>30</v>
+      </c>
+      <c r="L6" s="17">
+        <v>10.922800000000001</v>
+      </c>
+      <c r="M6" s="22">
+        <f>K6/L6</f>
+        <v>2.7465485040465811</v>
+      </c>
+      <c r="N6" s="17">
+        <v>6300</v>
+      </c>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17">
+        <v>30</v>
+      </c>
+      <c r="H7" s="17">
+        <v>62</v>
+      </c>
+      <c r="I7" s="17">
+        <v>23.8</v>
+      </c>
+      <c r="J7" s="17">
+        <v>30.5</v>
+      </c>
+      <c r="K7" s="17">
+        <v>22</v>
+      </c>
+      <c r="L7" s="17">
+        <v>10.922800000000001</v>
+      </c>
+      <c r="M7" s="22">
+        <f t="shared" ref="M7:M8" si="0">K7/L7</f>
+        <v>2.0141355696341599</v>
+      </c>
+      <c r="N7" s="17">
+        <v>7500</v>
+      </c>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="20">
+        <v>14.15</v>
+      </c>
+      <c r="G8" s="17">
+        <v>30</v>
+      </c>
+      <c r="H8" s="17">
+        <v>72</v>
+      </c>
+      <c r="I8" s="17">
+        <v>19</v>
+      </c>
+      <c r="J8" s="17">
+        <v>29.6</v>
+      </c>
+      <c r="K8" s="17">
+        <v>16</v>
+      </c>
+      <c r="L8" s="17">
+        <v>3.2700999999999998</v>
+      </c>
+      <c r="M8" s="22">
+        <f t="shared" si="0"/>
+        <v>4.8928167334332286</v>
+      </c>
+      <c r="N8" s="17">
+        <v>6300</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N3:N8">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="6100"/>
+        <cfvo type="num" val="6100"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{65131E50-8B69-4F61-BA4B-0451CFF26482}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{97E11B02-559F-4BB5-B2B7-782B97DEEB04}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{44DEAE0E-723D-4FD8-81EE-57D3BEFC1992}"/>
+    <hyperlink ref="D8" r:id="rId4" display="https://www.skf.com/in/products/rolling-bearings/ball-bearings/deep-groove-ball-bearings/productid-6306-2RS1" xr:uid="{0FBD705D-FECC-4B38-A6B3-FC7B6F12910D}"/>
+    <hyperlink ref="E8" r:id="rId5" display="https://uk.rs-online.com/web/p/ball-bearings/2851103" xr:uid="{E551C1A4-EC33-4816-902D-010290AD73FE}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{A04DDDE5-CB20-4A65-943E-459E4467449D}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{17E5E404-4237-4B7C-93B2-0F998C8C4018}"/>
+    <hyperlink ref="E3" r:id="rId8" xr:uid="{6B0D4912-9E13-45AF-92AE-C866BE7D690D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId9"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,11 +2057,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1909DA-F803-4A95-BDC3-3A661989B98E}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1241,7 +2108,7 @@
       <c r="D2">
         <v>27</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2">
         <v>30.378</v>
       </c>
       <c r="F2">
@@ -1262,7 +2129,7 @@
       <c r="D3">
         <v>19</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3">
         <v>167.078</v>
       </c>
       <c r="F3">
@@ -1280,7 +2147,7 @@
       <c r="D4">
         <v>48</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4">
         <v>82.878</v>
       </c>
       <c r="F4">

</xml_diff>

<commit_message>
update with latest dimensions from CAD
</commit_message>
<xml_diff>
--- a/Bearing Choices.xlsx
+++ b/Bearing Choices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsoep\OUR\Bearing_Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83B8A8-F4B5-4DFC-B16F-A0251B1C6AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2DE342-8A6F-4A4A-8BAF-41233727E47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bearing choices" sheetId="3" r:id="rId1"/>
@@ -1288,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D89061-B20F-468F-AF91-469D4018105C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,11 +1407,11 @@
         <v>38</v>
       </c>
       <c r="L3" s="17">
-        <v>10.922800000000001</v>
+        <v>9.9644999999999992</v>
       </c>
       <c r="M3" s="22">
         <f t="shared" ref="M3:M8" si="0">K3/L3</f>
-        <v>3.4789614384590029</v>
+        <v>3.813538060113403</v>
       </c>
       <c r="N3" s="17">
         <v>8500</v>
@@ -1453,11 +1453,11 @@
         <v>38</v>
       </c>
       <c r="L4" s="17">
-        <v>10.922800000000001</v>
+        <v>9.9644999999999992</v>
       </c>
       <c r="M4" s="22">
         <f t="shared" si="0"/>
-        <v>3.4789614384590029</v>
+        <v>3.813538060113403</v>
       </c>
       <c r="N4" s="17">
         <v>6000</v>
@@ -1499,11 +1499,11 @@
         <v>30</v>
       </c>
       <c r="L5" s="17">
-        <v>10.922800000000001</v>
+        <v>9.9644999999999992</v>
       </c>
       <c r="M5" s="22">
         <f t="shared" si="0"/>
-        <v>2.7465485040465811</v>
+        <v>3.0106879421947919</v>
       </c>
       <c r="N5" s="17">
         <v>6300</v>
@@ -1547,11 +1547,11 @@
         <v>30</v>
       </c>
       <c r="L6" s="17">
-        <v>10.922800000000001</v>
+        <v>9.9644999999999992</v>
       </c>
       <c r="M6" s="22">
         <f t="shared" si="0"/>
-        <v>2.7465485040465811</v>
+        <v>3.0106879421947919</v>
       </c>
       <c r="N6" s="17">
         <v>6300</v>
@@ -1593,11 +1593,11 @@
         <v>22</v>
       </c>
       <c r="L7" s="17">
-        <v>10.922800000000001</v>
+        <v>9.9644999999999992</v>
       </c>
       <c r="M7" s="22">
         <f t="shared" si="0"/>
-        <v>2.0141355696341599</v>
+        <v>2.2078378242761807</v>
       </c>
       <c r="N7" s="17">
         <v>7500</v>
@@ -1639,11 +1639,11 @@
         <v>16</v>
       </c>
       <c r="L8" s="17">
-        <v>3.2700999999999998</v>
+        <v>2.3117999999999999</v>
       </c>
       <c r="M8" s="22">
         <f t="shared" si="0"/>
-        <v>4.8928167334332286</v>
+        <v>6.9210139285405319</v>
       </c>
       <c r="N8" s="17">
         <v>6300</v>

</xml_diff>